<commit_message>
removed some bugs from the pdf creation code
</commit_message>
<xml_diff>
--- a/scripts/excel.xlsx
+++ b/scripts/excel.xlsx
@@ -47,7 +47,7 @@
     <t>Price</t>
   </si>
   <si>
-    <t>2017 Abarth 124 SPIDER ▲</t>
+    <t>2017 Abarth 124 SPIDER </t>
   </si>
   <si>
     <t>C</t>
@@ -68,7 +68,7 @@
     <t>43,500</t>
   </si>
   <si>
-    <t>2014 Alfa Romeo 4C ▲</t>
+    <t>2014 Alfa Romeo 4C </t>
   </si>
   <si>
     <t>A</t>
@@ -86,7 +86,7 @@
     <t>74,000</t>
   </si>
   <si>
-    <t>2017 Alpine A110 ▲</t>
+    <t>2017 Alpine A110 </t>
   </si>
   <si>
     <t>740</t>
@@ -101,7 +101,7 @@
     <t>HTF(250,000)</t>
   </si>
   <si>
-    <t>2016 Abarth 695 BIPOSTO ▲</t>
+    <t>2016 Abarth 695 BIPOSTO </t>
   </si>
   <si>
     <t>B</t>
@@ -122,7 +122,7 @@
     <t>48,000</t>
   </si>
   <si>
-    <t>1980 Abarth FIAT 131 ▲</t>
+    <t>1980 Abarth FIAT 131 </t>
   </si>
   <si>
     <t>D</t>
@@ -140,7 +140,7 @@
     <t>38,000</t>
   </si>
   <si>
-    <t>1968 Abarth 595 ESSEESSE ▲</t>
+    <t>1968 Abarth 595 ESSEESSE </t>
   </si>
   <si>
     <t>100</t>
@@ -155,7 +155,7 @@
     <t>35,000</t>
   </si>
   <si>
-    <t>2017 Acura NSX ▲</t>
+    <t>2017 Acura NSX </t>
   </si>
   <si>
     <t>S1</t>
@@ -176,7 +176,7 @@
     <t>170,000</t>
   </si>
   <si>
-    <t>2002 Acura RSX TYPE-S ▲</t>
+    <t>2002 Acura RSX TYPE-S </t>
   </si>
   <si>
     <t>588</t>
@@ -191,7 +191,7 @@
     <t>25,000</t>
   </si>
   <si>
-    <t>2001 Acura INTEGRA TYPE-R ▲</t>
+    <t>2001 Acura INTEGRA TYPE-R </t>
   </si>
   <si>
     <t>596</t>
@@ -203,7 +203,7 @@
     <t>2,639 lbs</t>
   </si>
   <si>
-    <t>2018 Alfa Romeo STELVIO QUADRIFOGLIO ▲</t>
+    <t>2018 Alfa Romeo STELVIO QUADRIFOGLIO </t>
   </si>
   <si>
     <t>752</t>
@@ -218,7 +218,7 @@
     <t>80,000</t>
   </si>
   <si>
-    <t>2017 Alfa Romeo GIULIA QUADRIFOGLIO ▲</t>
+    <t>2017 Alfa Romeo GIULIA QUADRIFOGLIO </t>
   </si>
   <si>
     <t>795</t>
@@ -233,7 +233,7 @@
     <t>120,000</t>
   </si>
   <si>
-    <t>2016 Alfa Romeo GIULIA QUADRIFOGLIO FORZA EDITION ▲</t>
+    <t>2016 Alfa Romeo GIULIA QUADRIFOGLIO FORZA EDITION </t>
   </si>
   <si>
     <t>812</t>
@@ -245,7 +245,7 @@
     <t>370,000</t>
   </si>
   <si>
-    <t>2007 Alfa Romeo 8C COMPETIZIONE ▲</t>
+    <t>2007 Alfa Romeo 8C COMPETIZIONE </t>
   </si>
   <si>
     <t>777</t>
@@ -260,7 +260,7 @@
     <t>300,000</t>
   </si>
   <si>
-    <t>2007 Alfa Romeo 8C COMPETIZIONE FORZA EDITION ▲</t>
+    <t>2007 Alfa Romeo 8C COMPETIZIONE FORZA EDITION </t>
   </si>
   <si>
     <t>855</t>
@@ -272,7 +272,7 @@
     <t>550,000</t>
   </si>
   <si>
-    <t>1992 Alfa Romeo 155 Q4 ▲</t>
+    <t>1992 Alfa Romeo 155 Q4 </t>
   </si>
   <si>
     <t>541</t>
@@ -281,7 +281,7 @@
     <t>3,064 lbs</t>
   </si>
   <si>
-    <t>1968 Alfa Romeo 33 STRADALE ▲</t>
+    <t>1968 Alfa Romeo 33 STRADALE </t>
   </si>
   <si>
     <t>716</t>
@@ -296,7 +296,7 @@
     <t>10,000,000</t>
   </si>
   <si>
-    <t>1965 Alfa Romeo GIULIA TZ2 ▲</t>
+    <t>1965 Alfa Romeo GIULIA TZ2 </t>
   </si>
   <si>
     <t>639</t>
@@ -311,7 +311,7 @@
     <t>2,500,000</t>
   </si>
   <si>
-    <t>1965 Alfa Romeo GIULIA SPRINT GTA STRADALE ▲</t>
+    <t>1965 Alfa Romeo GIULIA SPRINT GTA STRADALE </t>
   </si>
   <si>
     <t>432</t>
@@ -323,7 +323,7 @@
     <t>1,676 lbs</t>
   </si>
   <si>
-    <t>1934 Alfa Romeo P3 ▲</t>
+    <t>1934 Alfa Romeo P3 </t>
   </si>
   <si>
     <t>626</t>
@@ -335,7 +335,7 @@
     <t>1,653 lbs</t>
   </si>
   <si>
-    <t>2015 Alumi Craft CLASS 10 RACE CAR ▲</t>
+    <t>2015 Alumi Craft CLASS 10 RACE CAR </t>
   </si>
   <si>
     <t>673</t>

</xml_diff>